<commit_message>
edited gantt + made ai class
ai does not do anything yet
</commit_message>
<xml_diff>
--- a/Documents/Gantt Chart/Trajectory_Gantt_2.0.xlsx
+++ b/Documents/Gantt Chart/Trajectory_Gantt_2.0.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a98965/Dropbox/CS383/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Satan\Documents\GitHub\Trajectory\Documents\Gantt Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5168AF51-F50B-7943-8EC3-9064A9769D9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4E8E0F0-78AC-4CC9-8213-94CF5CE56F08}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16680" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Management Summary" sheetId="3" r:id="rId1"/>
@@ -27,9 +27,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,10 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="117">
-  <si>
-    <t>planned</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="112">
   <si>
     <t>Meetings</t>
   </si>
@@ -198,21 +193,9 @@
     <t>Developing Tests</t>
   </si>
   <si>
-    <t>Sound/Music Collection</t>
-  </si>
-  <si>
-    <t>Event Decode</t>
-  </si>
-  <si>
-    <t>Audio Control</t>
-  </si>
-  <si>
     <t>Testing</t>
   </si>
   <si>
-    <t>Merging</t>
-  </si>
-  <si>
     <t>Noah Mammen</t>
   </si>
   <si>
@@ -378,9 +361,6 @@
     <t>F Research into AI</t>
   </si>
   <si>
-    <t>Max Icardo (Left team)</t>
-  </si>
-  <si>
     <t>Mar 31th</t>
   </si>
   <si>
@@ -388,6 +368,9 @@
   </si>
   <si>
     <t>In progess</t>
+  </si>
+  <si>
+    <t>Progress</t>
   </si>
 </sst>
 </file>
@@ -668,7 +651,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -753,6 +736,8 @@
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -765,8 +750,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1087,106 +1071,106 @@
       <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="3" max="3" width="14.33203125" customWidth="1"/>
-    <col min="4" max="4" width="13.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.77734375" customWidth="1"/>
     <col min="5" max="5" width="13.33203125" customWidth="1"/>
-    <col min="6" max="6" width="3.5" customWidth="1"/>
+    <col min="6" max="6" width="3.44140625" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" customWidth="1"/>
     <col min="8" max="8" width="12.33203125" customWidth="1"/>
-    <col min="9" max="9" width="14.5" customWidth="1"/>
-    <col min="10" max="10" width="2.83203125" customWidth="1"/>
-    <col min="11" max="11" width="13.83203125" customWidth="1"/>
+    <col min="9" max="9" width="14.44140625" customWidth="1"/>
+    <col min="10" max="10" width="2.77734375" customWidth="1"/>
+    <col min="11" max="11" width="13.77734375" customWidth="1"/>
     <col min="12" max="12" width="14" customWidth="1"/>
-    <col min="13" max="13" width="14.1640625" customWidth="1"/>
-    <col min="14" max="14" width="5.5" customWidth="1"/>
+    <col min="13" max="13" width="14.109375" customWidth="1"/>
+    <col min="14" max="14" width="5.44140625" customWidth="1"/>
     <col min="15" max="15" width="12.33203125" customWidth="1"/>
     <col min="16" max="16" width="14.6640625" customWidth="1"/>
     <col min="17" max="17" width="11.33203125" customWidth="1"/>
     <col min="19" max="21" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:21" ht="16" thickBot="1"/>
+    <row r="1" spans="2:21" ht="15" thickBot="1"/>
     <row r="2" spans="2:21">
-      <c r="C2" s="70" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="71"/>
-      <c r="E2" s="72"/>
+      <c r="C2" s="72" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="73"/>
+      <c r="E2" s="74"/>
       <c r="F2" s="8"/>
-      <c r="G2" s="70" t="s">
+      <c r="G2" s="72" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="73"/>
+      <c r="I2" s="74"/>
+      <c r="K2" s="72" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="73"/>
+      <c r="M2" s="74"/>
+      <c r="O2" s="72" t="s">
+        <v>17</v>
+      </c>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="74"/>
+      <c r="S2" s="72" t="s">
+        <v>84</v>
+      </c>
+      <c r="T2" s="73"/>
+      <c r="U2" s="74"/>
+    </row>
+    <row r="3" spans="2:21" ht="15" thickBot="1">
+      <c r="C3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="11" t="s">
         <v>10</v>
-      </c>
-      <c r="H2" s="71"/>
-      <c r="I2" s="72"/>
-      <c r="K2" s="70" t="s">
-        <v>1</v>
-      </c>
-      <c r="L2" s="71"/>
-      <c r="M2" s="72"/>
-      <c r="O2" s="70" t="s">
-        <v>18</v>
-      </c>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="72"/>
-      <c r="S2" s="70" t="s">
-        <v>89</v>
-      </c>
-      <c r="T2" s="71"/>
-      <c r="U2" s="72"/>
-    </row>
-    <row r="3" spans="2:21" ht="16" thickBot="1">
-      <c r="C3" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>11</v>
       </c>
       <c r="F3" s="1"/>
       <c r="G3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="13" t="s">
-        <v>9</v>
-      </c>
       <c r="I3" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="K3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="13" t="s">
-        <v>9</v>
-      </c>
       <c r="M3" s="14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="O3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="P3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="P3" s="10" t="s">
-        <v>9</v>
-      </c>
       <c r="Q3" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="S3" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="T3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="T3" s="10" t="s">
-        <v>9</v>
-      </c>
       <c r="U3" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="2:21" ht="16" thickBot="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="2:21" ht="15" thickBot="1">
       <c r="B4" s="25" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C4" s="22">
         <f>(G4+K4 +O4)</f>
@@ -1249,9 +1233,9 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="5" spans="2:21" ht="16" thickBot="1">
+    <row r="5" spans="2:21" ht="15" thickBot="1">
       <c r="B5" s="9" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C5" s="16">
         <f t="shared" ref="C5:C7" si="0">(G5+K5 +O5)</f>
@@ -1314,9 +1298,9 @@
         <v>800</v>
       </c>
     </row>
-    <row r="6" spans="2:21" ht="16" thickBot="1">
+    <row r="6" spans="2:21" ht="15" thickBot="1">
       <c r="B6" s="9" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C6" s="16">
         <f t="shared" si="0"/>
@@ -1324,24 +1308,24 @@
       </c>
       <c r="D6" s="17">
         <f>(H6+L6 +P6+T4)</f>
-        <v>5900</v>
+        <v>6700</v>
       </c>
       <c r="E6" s="18">
         <f t="shared" si="1"/>
-        <v>3400</v>
+        <v>2600</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="16">
-        <f>(Gantt!F46)*100</f>
+        <f>(Gantt!F39)*100</f>
         <v>4800</v>
       </c>
       <c r="H6" s="17">
-        <f>(Gantt!G46)*100</f>
-        <v>1400</v>
+        <f>(Gantt!G39)*100</f>
+        <v>2200</v>
       </c>
       <c r="I6" s="18">
         <f t="shared" si="2"/>
-        <v>3400</v>
+        <v>2600</v>
       </c>
       <c r="K6" s="16">
         <v>1000</v>
@@ -1379,9 +1363,9 @@
         <v>1600</v>
       </c>
     </row>
-    <row r="7" spans="2:21" ht="16" thickBot="1">
+    <row r="7" spans="2:21" ht="15" thickBot="1">
       <c r="B7" s="9" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C7" s="47">
         <f t="shared" si="0"/>
@@ -1397,11 +1381,11 @@
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="16">
-        <f>(Gantt!F56)*100</f>
+        <f>(Gantt!F49)*100</f>
         <v>6600</v>
       </c>
       <c r="H7" s="17">
-        <f>(Gantt!G56)*100</f>
+        <f>(Gantt!G49)*100</f>
         <v>3000</v>
       </c>
       <c r="I7" s="18">
@@ -1444,9 +1428,9 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="8" spans="2:21" ht="16" thickBot="1">
+    <row r="8" spans="2:21" ht="15" thickBot="1">
       <c r="B8" s="15" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C8" s="26">
         <f>SUM(C4:C7)</f>
@@ -1454,11 +1438,11 @@
       </c>
       <c r="D8" s="27">
         <f>SUM(D4:D7)</f>
-        <v>22150</v>
+        <v>22950</v>
       </c>
       <c r="E8" s="28">
         <f>SUM(E4:E7)</f>
-        <v>14150</v>
+        <v>13350</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="19">
@@ -1467,11 +1451,11 @@
       </c>
       <c r="H8" s="20">
         <f>SUM(H4:H7)</f>
-        <v>6550</v>
+        <v>7350</v>
       </c>
       <c r="I8" s="21">
         <f>SUM(I4:I7)</f>
-        <v>12450</v>
+        <v>11650</v>
       </c>
       <c r="K8" s="19">
         <f>SUM(K4:K7)</f>
@@ -1512,7 +1496,7 @@
     </row>
     <row r="10" spans="2:21">
       <c r="B10" s="10" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1532,48 +1516,48 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BQ57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="125" zoomScaleNormal="191" workbookViewId="0">
-      <selection activeCell="Z9" sqref="Z9:AA9"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="125" zoomScaleNormal="191" workbookViewId="0">
+      <selection activeCell="I34" sqref="I34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="17.5" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" customWidth="1"/>
     <col min="3" max="3" width="15.6640625" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" ht="16">
+    <row r="1" spans="1:68" ht="15.6">
       <c r="A1" s="50" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E1" s="50" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F1" s="50"/>
       <c r="G1" s="50" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="50" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="50" t="s">
+      <c r="I1" s="51" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="51" t="s">
+      <c r="J1" s="52" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="52" t="s">
+      <c r="K1" s="53" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="53" t="s">
+      <c r="L1" s="54" t="s">
         <v>25</v>
-      </c>
-      <c r="L1" s="54" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:68">
       <c r="A2" s="55" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" s="55"/>
       <c r="C2" s="55"/>
@@ -1765,7 +1749,7 @@
     </row>
     <row r="3" spans="1:68">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3">
         <v>1</v>
@@ -1776,14 +1760,14 @@
       <c r="G3">
         <v>1</v>
       </c>
-      <c r="H3" s="74" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="74"/>
+      <c r="H3" s="70" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="70"/>
     </row>
     <row r="4" spans="1:68">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E4">
         <v>2</v>
@@ -1795,7 +1779,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="53" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="J4" s="61">
         <v>1</v>
@@ -1818,7 +1802,7 @@
     </row>
     <row r="5" spans="1:68">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5">
         <v>3</v>
@@ -1830,7 +1814,7 @@
         <v>1</v>
       </c>
       <c r="H5" s="52" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="J5" s="58">
         <v>1</v>
@@ -1842,7 +1826,7 @@
     </row>
     <row r="6" spans="1:68">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -1851,7 +1835,7 @@
         <v>5</v>
       </c>
       <c r="H6" s="56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="O6" s="57">
         <v>3</v>
@@ -1863,7 +1847,7 @@
     </row>
     <row r="7" spans="1:68">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7">
         <v>5</v>
@@ -1872,7 +1856,7 @@
         <v>4</v>
       </c>
       <c r="H7" s="56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="T7" s="57">
         <v>4</v>
@@ -1883,7 +1867,7 @@
     </row>
     <row r="8" spans="1:68">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8">
         <v>6</v>
@@ -1894,8 +1878,8 @@
       <c r="G8">
         <v>1.5</v>
       </c>
-      <c r="H8" s="75" t="s">
-        <v>116</v>
+      <c r="H8" s="71" t="s">
+        <v>110</v>
       </c>
       <c r="X8" s="58">
         <v>5</v>
@@ -1904,7 +1888,7 @@
     </row>
     <row r="9" spans="1:68">
       <c r="A9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9">
         <v>7</v>
@@ -1915,17 +1899,17 @@
       <c r="G9">
         <v>1</v>
       </c>
-      <c r="H9" s="75" t="s">
-        <v>116</v>
+      <c r="H9" s="71" t="s">
+        <v>110</v>
       </c>
       <c r="Z9" s="52" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AA9" s="52"/>
     </row>
     <row r="10" spans="1:68">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E10">
         <v>8</v>
@@ -1934,7 +1918,7 @@
         <v>5</v>
       </c>
       <c r="H10" s="56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AB10" s="57">
         <v>7</v>
@@ -1946,7 +1930,7 @@
     </row>
     <row r="11" spans="1:68">
       <c r="A11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E11">
         <v>9</v>
@@ -1955,7 +1939,7 @@
         <v>3</v>
       </c>
       <c r="H11" s="56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AG11" s="57">
         <v>8</v>
@@ -1965,7 +1949,7 @@
     </row>
     <row r="12" spans="1:68">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F12">
         <f>SUM(F3:F11)</f>
@@ -1978,7 +1962,7 @@
     </row>
     <row r="13" spans="1:68">
       <c r="A13" s="55" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B13" s="55"/>
       <c r="C13" s="55"/>
@@ -2042,7 +2026,7 @@
     </row>
     <row r="14" spans="1:68">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E14">
         <v>1</v>
@@ -2054,14 +2038,14 @@
         <v>2</v>
       </c>
       <c r="H14" s="53" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I14" s="53"/>
       <c r="J14" s="53"/>
     </row>
     <row r="15" spans="1:68">
       <c r="A15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E15">
         <v>2</v>
@@ -2073,14 +2057,14 @@
         <v>2</v>
       </c>
       <c r="H15" s="53" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I15" s="53"/>
       <c r="J15" s="53"/>
     </row>
     <row r="16" spans="1:68">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E16">
         <v>3</v>
@@ -2092,14 +2076,14 @@
         <v>2</v>
       </c>
       <c r="H16" s="53" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="I16" s="53"/>
       <c r="J16" s="53"/>
     </row>
     <row r="17" spans="1:69">
       <c r="A17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E17">
         <v>4</v>
@@ -2111,10 +2095,10 @@
         <v>3</v>
       </c>
       <c r="H17" s="52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="K17" s="52" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L17" s="52"/>
       <c r="M17" s="52"/>
@@ -2122,7 +2106,7 @@
     </row>
     <row r="18" spans="1:69">
       <c r="A18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E18">
         <v>5</v>
@@ -2134,7 +2118,7 @@
         <v>2</v>
       </c>
       <c r="H18" s="52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O18" s="58">
         <v>4</v>
@@ -2150,7 +2134,7 @@
     </row>
     <row r="19" spans="1:69">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E19">
         <v>6</v>
@@ -2162,7 +2146,7 @@
         <v>2</v>
       </c>
       <c r="H19" s="52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="O19" s="58">
         <v>4</v>
@@ -2172,7 +2156,7 @@
     </row>
     <row r="20" spans="1:69">
       <c r="A20" s="59" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20" s="59"/>
       <c r="C20" s="59"/>
@@ -2187,7 +2171,7 @@
         <v>1</v>
       </c>
       <c r="H20" s="52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="R20" s="58">
         <v>6</v>
@@ -2200,7 +2184,7 @@
     </row>
     <row r="21" spans="1:69">
       <c r="A21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="E21">
         <v>8</v>
@@ -2212,10 +2196,10 @@
         <v>2</v>
       </c>
       <c r="H21" s="52" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="X21" s="58" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="Y21" s="58"/>
       <c r="Z21" s="58"/>
@@ -2225,7 +2209,7 @@
     </row>
     <row r="22" spans="1:69">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E22">
         <v>9</v>
@@ -2234,7 +2218,7 @@
         <v>6</v>
       </c>
       <c r="H22" s="56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="AD22" s="57">
         <v>8</v>
@@ -2247,7 +2231,7 @@
     </row>
     <row r="23" spans="1:69">
       <c r="A23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E23">
         <v>10</v>
@@ -2256,7 +2240,7 @@
         <v>6</v>
       </c>
       <c r="H23" s="56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="X23" s="57">
         <v>5</v>
@@ -2269,7 +2253,7 @@
     </row>
     <row r="24" spans="1:69">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E24">
         <v>11</v>
@@ -2278,7 +2262,7 @@
         <v>4</v>
       </c>
       <c r="H24" s="56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -2287,7 +2271,7 @@
     </row>
     <row r="25" spans="1:69">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E25">
         <v>12</v>
@@ -2296,7 +2280,7 @@
         <v>4</v>
       </c>
       <c r="H25" s="56" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -2305,7 +2289,7 @@
     </row>
     <row r="26" spans="1:69">
       <c r="A26" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F26">
         <f>SUM(F14:F25)</f>
@@ -2318,7 +2302,7 @@
     </row>
     <row r="27" spans="1:69">
       <c r="A27" s="55" t="s">
-        <v>113</v>
+        <v>53</v>
       </c>
       <c r="B27" s="55"/>
       <c r="C27" s="55"/>
@@ -2390,525 +2374,574 @@
       <c r="BQ27" s="55"/>
     </row>
     <row r="28" spans="1:69">
-      <c r="A28" t="s">
-        <v>53</v>
-      </c>
+      <c r="A28" s="75" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="75"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="75"/>
       <c r="E28">
         <v>1</v>
       </c>
       <c r="F28">
+        <v>4</v>
+      </c>
+      <c r="G28">
+        <v>4</v>
+      </c>
+      <c r="H28" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="I28" s="53"/>
+      <c r="J28" s="53"/>
+      <c r="K28" s="53"/>
+      <c r="L28" s="53"/>
+    </row>
+    <row r="29" spans="1:69">
+      <c r="A29" s="75" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="75"/>
+      <c r="C29" s="75"/>
+      <c r="D29" s="75"/>
+      <c r="E29">
+        <v>2</v>
+      </c>
+      <c r="F29">
+        <v>3</v>
+      </c>
+      <c r="G29">
+        <v>3</v>
+      </c>
+      <c r="H29" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="M29" s="61">
         <v>1</v>
       </c>
-      <c r="H28" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="1:69">
-      <c r="A29" t="s">
-        <v>54</v>
-      </c>
-      <c r="E29">
-        <v>2</v>
-      </c>
-      <c r="F29">
-        <v>1</v>
-      </c>
-      <c r="H29" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="J29" s="57">
-        <v>1</v>
-      </c>
+      <c r="N29" s="53"/>
+      <c r="O29" s="61"/>
     </row>
     <row r="30" spans="1:69">
-      <c r="A30" t="s">
-        <v>55</v>
-      </c>
+      <c r="A30" s="75" t="s">
+        <v>56</v>
+      </c>
+      <c r="B30" s="75"/>
+      <c r="C30" s="75"/>
+      <c r="D30" s="75"/>
       <c r="E30">
         <v>3</v>
       </c>
       <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="H30" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="K30" s="57">
-        <v>2</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="G30">
+        <v>10</v>
+      </c>
+      <c r="H30" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="P30" s="61">
+        <v>2</v>
+      </c>
+      <c r="Q30" s="53"/>
+      <c r="R30" s="53"/>
+      <c r="S30" s="53"/>
+      <c r="T30" s="53"/>
+      <c r="U30" s="61"/>
+      <c r="V30" s="53"/>
+      <c r="W30" s="53"/>
+      <c r="X30" s="53"/>
+      <c r="Y30" s="53"/>
     </row>
     <row r="31" spans="1:69">
-      <c r="A31" t="s">
-        <v>56</v>
-      </c>
+      <c r="A31" s="75" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" s="75"/>
+      <c r="C31" s="75"/>
+      <c r="D31" s="75"/>
       <c r="E31">
         <v>4</v>
       </c>
       <c r="F31">
         <v>2</v>
       </c>
-      <c r="H31" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="L31" s="57">
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31" s="62" t="s">
+        <v>111</v>
+      </c>
+      <c r="Z31" s="58">
         <v>3</v>
       </c>
-      <c r="M31" s="2"/>
+      <c r="AA31" s="52"/>
     </row>
     <row r="32" spans="1:69">
-      <c r="A32" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="B32" s="59"/>
-      <c r="C32" s="59"/>
-      <c r="D32" s="59"/>
+      <c r="A32" s="75" t="s">
+        <v>58</v>
+      </c>
+      <c r="B32" s="75"/>
+      <c r="C32" s="75"/>
+      <c r="D32" s="75"/>
       <c r="E32">
         <v>5</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="64">
+        <v>3</v>
+      </c>
+      <c r="G32">
+        <v>2</v>
+      </c>
+      <c r="H32" s="60" t="s">
+        <v>24</v>
+      </c>
+      <c r="I32" s="53"/>
+      <c r="J32" s="53"/>
+      <c r="K32" s="53"/>
+    </row>
+    <row r="33" spans="1:69">
+      <c r="A33" s="75" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="75"/>
+      <c r="C33" s="75"/>
+      <c r="D33" s="75"/>
+      <c r="E33">
+        <v>6</v>
+      </c>
+      <c r="F33">
+        <v>4</v>
+      </c>
+      <c r="G33">
+        <v>2</v>
+      </c>
+      <c r="H33" s="62" t="s">
+        <v>111</v>
+      </c>
+      <c r="L33" s="58">
+        <v>5</v>
+      </c>
+      <c r="M33" s="52"/>
+      <c r="N33" s="52"/>
+      <c r="O33" s="52"/>
+      <c r="P33" s="76"/>
+      <c r="Q33" s="76"/>
+      <c r="R33" s="76"/>
+      <c r="S33" s="76"/>
+      <c r="T33" s="76"/>
+      <c r="U33" s="76"/>
+      <c r="V33" s="76"/>
+      <c r="W33" s="76"/>
+      <c r="X33" s="76"/>
+      <c r="Y33" s="76"/>
+    </row>
+    <row r="34" spans="1:69">
+      <c r="A34" s="75" t="s">
+        <v>60</v>
+      </c>
+      <c r="B34" s="75"/>
+      <c r="C34" s="75"/>
+      <c r="D34" s="75"/>
+      <c r="E34">
+        <v>7</v>
+      </c>
+      <c r="F34">
+        <v>10</v>
+      </c>
+      <c r="H34" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z34" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA34" s="2"/>
+      <c r="AB34" s="2"/>
+      <c r="AC34" s="2"/>
+      <c r="AD34" s="2"/>
+      <c r="AE34" s="2"/>
+      <c r="AF34" s="2"/>
+      <c r="AG34" s="2"/>
+      <c r="AH34" s="2"/>
+      <c r="AI34" s="2"/>
+    </row>
+    <row r="35" spans="1:69">
+      <c r="A35" s="75" t="s">
+        <v>62</v>
+      </c>
+      <c r="B35" s="75"/>
+      <c r="C35" s="75"/>
+      <c r="D35" s="75"/>
+      <c r="E35">
+        <v>8</v>
+      </c>
+      <c r="F35">
+        <v>3</v>
+      </c>
+      <c r="H35" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="AJ35" s="2"/>
+      <c r="AK35" s="2"/>
+      <c r="AL35" s="2"/>
+      <c r="AR35" s="59"/>
+    </row>
+    <row r="36" spans="1:69">
+      <c r="A36" s="75" t="s">
+        <v>52</v>
+      </c>
+      <c r="B36" s="75"/>
+      <c r="C36" s="75"/>
+      <c r="D36" s="75"/>
+      <c r="E36">
+        <v>9</v>
+      </c>
+      <c r="F36">
+        <v>4</v>
+      </c>
+      <c r="H36" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="AM36" s="2"/>
+      <c r="AN36" s="2"/>
+      <c r="AO36" s="2"/>
+      <c r="AP36" s="2"/>
+      <c r="AR36" s="59"/>
+    </row>
+    <row r="37" spans="1:69">
+      <c r="A37" s="75" t="s">
+        <v>63</v>
+      </c>
+      <c r="B37" s="75"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
+      <c r="E37">
+        <v>10</v>
+      </c>
+      <c r="F37">
+        <v>2</v>
+      </c>
+      <c r="H37" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="AQ37" s="2"/>
+      <c r="AR37" s="57"/>
+    </row>
+    <row r="38" spans="1:69">
+      <c r="A38" s="75" t="s">
+        <v>64</v>
+      </c>
+      <c r="B38" s="75"/>
+      <c r="C38" s="75"/>
+      <c r="D38" s="75"/>
+      <c r="E38">
+        <v>11</v>
+      </c>
+      <c r="F38">
+        <v>3</v>
+      </c>
+      <c r="H38" s="63" t="s">
+        <v>22</v>
+      </c>
+      <c r="AS38" s="2"/>
+      <c r="AT38" s="2"/>
+      <c r="AU38" s="2"/>
+    </row>
+    <row r="39" spans="1:69">
+      <c r="A39" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="H32" s="56" t="s">
-        <v>0</v>
-      </c>
-      <c r="N32" s="57">
+      <c r="B39" s="59"/>
+      <c r="C39" s="59"/>
+      <c r="D39" s="59"/>
+      <c r="F39">
+        <f>SUM(F28:F38)</f>
+        <v>48</v>
+      </c>
+      <c r="G39">
+        <f>SUM(G28:G38)</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" spans="1:69">
+      <c r="A40" s="55" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" s="55"/>
+      <c r="C40" s="55"/>
+      <c r="D40" s="55"/>
+      <c r="E40" s="55"/>
+      <c r="F40" s="55"/>
+      <c r="G40" s="55"/>
+      <c r="H40" s="55"/>
+      <c r="I40" s="55"/>
+      <c r="J40" s="55"/>
+      <c r="K40" s="55"/>
+      <c r="L40" s="55"/>
+      <c r="M40" s="55"/>
+      <c r="N40" s="55"/>
+      <c r="O40" s="55"/>
+      <c r="P40" s="55"/>
+      <c r="Q40" s="55"/>
+      <c r="R40" s="55"/>
+      <c r="S40" s="55"/>
+      <c r="T40" s="55"/>
+      <c r="U40" s="55"/>
+      <c r="V40" s="55"/>
+      <c r="W40" s="55"/>
+      <c r="X40" s="55"/>
+      <c r="Y40" s="55"/>
+      <c r="Z40" s="55"/>
+      <c r="AA40" s="55"/>
+      <c r="AB40" s="55"/>
+      <c r="AC40" s="55"/>
+      <c r="AD40" s="55"/>
+      <c r="AE40" s="55"/>
+      <c r="AF40" s="55"/>
+      <c r="AG40" s="55"/>
+      <c r="AH40" s="55"/>
+      <c r="AI40" s="55"/>
+      <c r="AJ40" s="55"/>
+      <c r="AK40" s="55"/>
+      <c r="AL40" s="55"/>
+      <c r="AM40" s="55"/>
+      <c r="AN40" s="55"/>
+      <c r="AO40" s="55"/>
+      <c r="AP40" s="55"/>
+      <c r="AQ40" s="55"/>
+      <c r="AR40" s="55"/>
+      <c r="AS40" s="55"/>
+      <c r="AT40" s="55"/>
+      <c r="AU40" s="55"/>
+      <c r="AV40" s="55"/>
+      <c r="AW40" s="55"/>
+      <c r="AX40" s="55"/>
+      <c r="AY40" s="55"/>
+      <c r="AZ40" s="55"/>
+      <c r="BA40" s="55"/>
+      <c r="BB40" s="55"/>
+      <c r="BC40" s="55"/>
+      <c r="BD40" s="55"/>
+      <c r="BE40" s="55"/>
+      <c r="BF40" s="55"/>
+      <c r="BG40" s="55"/>
+      <c r="BH40" s="55"/>
+      <c r="BI40" s="55"/>
+      <c r="BJ40" s="55"/>
+      <c r="BK40" s="55"/>
+      <c r="BL40" s="55"/>
+      <c r="BM40" s="55"/>
+    </row>
+    <row r="41" spans="1:69">
+      <c r="A41" s="59" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" s="59"/>
+      <c r="C41" s="59"/>
+      <c r="D41" s="59"/>
+      <c r="E41">
+        <v>1</v>
+      </c>
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="I41" s="53"/>
+    </row>
+    <row r="42" spans="1:69">
+      <c r="A42" s="59" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" s="59"/>
+      <c r="C42" s="59"/>
+      <c r="D42" s="59"/>
+      <c r="E42">
+        <v>2</v>
+      </c>
+      <c r="F42">
+        <v>2</v>
+      </c>
+      <c r="G42">
+        <v>2</v>
+      </c>
+      <c r="H42" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="J42" s="61">
+        <v>1</v>
+      </c>
+      <c r="K42" s="53"/>
+    </row>
+    <row r="43" spans="1:69">
+      <c r="A43" s="59" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" s="59"/>
+      <c r="C43" s="59"/>
+      <c r="D43" s="59"/>
+      <c r="E43">
+        <v>3</v>
+      </c>
+      <c r="F43">
+        <v>14</v>
+      </c>
+      <c r="G43">
+        <v>14</v>
+      </c>
+      <c r="H43" s="53" t="s">
+        <v>24</v>
+      </c>
+      <c r="L43" s="61">
+        <v>2</v>
+      </c>
+      <c r="M43" s="53"/>
+      <c r="N43" s="53"/>
+      <c r="O43" s="53"/>
+      <c r="P43" s="53"/>
+      <c r="Q43" s="53"/>
+      <c r="R43" s="53"/>
+      <c r="S43" s="53"/>
+      <c r="T43" s="53"/>
+      <c r="U43" s="53"/>
+      <c r="V43" s="53"/>
+      <c r="W43" s="53"/>
+      <c r="X43" s="53"/>
+      <c r="Y43" s="53"/>
+    </row>
+    <row r="44" spans="1:69">
+      <c r="A44" s="59" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" s="59"/>
+      <c r="C44" s="59"/>
+      <c r="D44" s="59"/>
+      <c r="E44">
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:69">
-      <c r="A33" t="s">
-        <v>2</v>
-      </c>
-      <c r="F33">
-        <v>6</v>
-      </c>
-      <c r="G33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:69">
-      <c r="A34" s="55" t="s">
-        <v>58</v>
-      </c>
-      <c r="B34" s="55"/>
-      <c r="C34" s="55"/>
-      <c r="D34" s="55"/>
-      <c r="E34" s="55"/>
-      <c r="F34" s="55"/>
-      <c r="G34" s="55"/>
-      <c r="H34" s="55"/>
-      <c r="I34" s="55"/>
-      <c r="J34" s="55"/>
-      <c r="K34" s="55"/>
-      <c r="L34" s="55"/>
-      <c r="M34" s="55"/>
-      <c r="N34" s="55"/>
-      <c r="O34" s="55"/>
-      <c r="P34" s="55"/>
-      <c r="Q34" s="55"/>
-      <c r="R34" s="55"/>
-      <c r="S34" s="55"/>
-      <c r="T34" s="55"/>
-      <c r="U34" s="55"/>
-      <c r="V34" s="55"/>
-      <c r="W34" s="55"/>
-      <c r="X34" s="55"/>
-      <c r="Y34" s="55"/>
-      <c r="Z34" s="55"/>
-      <c r="AA34" s="55"/>
-      <c r="AB34" s="55"/>
-      <c r="AC34" s="55"/>
-      <c r="AD34" s="55"/>
-      <c r="AE34" s="55"/>
-      <c r="AF34" s="55"/>
-      <c r="AG34" s="55"/>
-      <c r="AH34" s="55"/>
-      <c r="AI34" s="55"/>
-      <c r="AJ34" s="55"/>
-      <c r="AK34" s="55"/>
-      <c r="AL34" s="55"/>
-      <c r="AM34" s="55"/>
-      <c r="AN34" s="55"/>
-      <c r="AO34" s="55"/>
-      <c r="AP34" s="55"/>
-      <c r="AQ34" s="55"/>
-      <c r="AR34" s="55"/>
-      <c r="AS34" s="55"/>
-      <c r="AT34" s="55"/>
-      <c r="AU34" s="55"/>
-      <c r="AV34" s="55"/>
-      <c r="AW34" s="55"/>
-      <c r="AX34" s="55"/>
-      <c r="AY34" s="55"/>
-      <c r="AZ34" s="55"/>
-      <c r="BA34" s="55"/>
-      <c r="BB34" s="55"/>
-      <c r="BC34" s="55"/>
-      <c r="BD34" s="55"/>
-      <c r="BE34" s="55"/>
-      <c r="BF34" s="55"/>
-      <c r="BG34" s="55"/>
-      <c r="BH34" s="55"/>
-      <c r="BI34" s="55"/>
-      <c r="BJ34" s="55"/>
-      <c r="BK34" s="55"/>
-      <c r="BL34" s="55"/>
-      <c r="BM34" s="55"/>
-    </row>
-    <row r="35" spans="1:69">
-      <c r="A35" s="73" t="s">
-        <v>59</v>
-      </c>
-      <c r="B35" s="73"/>
-      <c r="C35" s="73"/>
-      <c r="D35" s="73"/>
-      <c r="E35">
-        <v>1</v>
-      </c>
-      <c r="F35">
-        <v>4</v>
-      </c>
-      <c r="G35">
-        <v>4</v>
-      </c>
-      <c r="H35" s="60" t="s">
-        <v>25</v>
-      </c>
-      <c r="I35" s="53"/>
-      <c r="J35" s="53"/>
-      <c r="K35" s="53"/>
-      <c r="L35" s="53"/>
-    </row>
-    <row r="36" spans="1:69">
-      <c r="A36" s="73" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" s="73"/>
-      <c r="C36" s="73"/>
-      <c r="D36" s="73"/>
-      <c r="E36">
-        <v>2</v>
-      </c>
-      <c r="F36">
+      <c r="F44">
+        <v>12</v>
+      </c>
+      <c r="G44">
+        <v>5</v>
+      </c>
+      <c r="H44" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z44" s="58">
         <v>3</v>
       </c>
-      <c r="G36">
+      <c r="AA44" s="52"/>
+      <c r="AB44" s="52"/>
+      <c r="AC44" s="52"/>
+      <c r="AD44" s="52"/>
+      <c r="AE44" s="52"/>
+      <c r="AF44" s="52"/>
+      <c r="AG44" s="52"/>
+      <c r="AH44" s="52"/>
+      <c r="AI44" s="52"/>
+      <c r="AJ44" s="52"/>
+      <c r="AK44" s="52"/>
+    </row>
+    <row r="45" spans="1:69">
+      <c r="A45" s="59" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" s="59"/>
+      <c r="C45" s="59"/>
+      <c r="D45" s="59"/>
+      <c r="E45">
+        <v>5</v>
+      </c>
+      <c r="F45">
+        <v>23</v>
+      </c>
+      <c r="G45">
+        <v>8</v>
+      </c>
+      <c r="H45" s="52" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z45" s="58">
         <v>3</v>
       </c>
-      <c r="H36" s="60" t="s">
-        <v>25</v>
-      </c>
-      <c r="M36" s="61">
-        <v>1</v>
-      </c>
-      <c r="N36" s="53"/>
-      <c r="O36" s="61"/>
-    </row>
-    <row r="37" spans="1:69">
-      <c r="A37" s="73" t="s">
-        <v>61</v>
-      </c>
-      <c r="B37" s="73"/>
-      <c r="C37" s="73"/>
-      <c r="D37" s="73"/>
-      <c r="E37">
-        <v>3</v>
-      </c>
-      <c r="F37">
-        <v>10</v>
-      </c>
-      <c r="G37">
-        <v>5</v>
-      </c>
-      <c r="H37" s="62" t="s">
-        <v>24</v>
-      </c>
-      <c r="P37" s="58">
-        <v>2</v>
-      </c>
-      <c r="Q37" s="52"/>
-      <c r="R37" s="52"/>
-      <c r="S37" s="52"/>
-      <c r="T37" s="52"/>
-      <c r="U37" s="58"/>
-      <c r="V37" s="52"/>
-      <c r="W37" s="52"/>
-      <c r="X37" s="52"/>
-      <c r="Y37" s="52"/>
-    </row>
-    <row r="38" spans="1:69">
-      <c r="A38" s="73" t="s">
-        <v>62</v>
-      </c>
-      <c r="B38" s="73"/>
-      <c r="C38" s="73"/>
-      <c r="D38" s="73"/>
-      <c r="E38">
-        <v>4</v>
-      </c>
-      <c r="F38">
-        <v>2</v>
-      </c>
-      <c r="H38" s="63" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z38" s="57">
-        <v>3</v>
-      </c>
-      <c r="AA38" s="2"/>
-    </row>
-    <row r="39" spans="1:69">
-      <c r="A39" s="73" t="s">
-        <v>63</v>
-      </c>
-      <c r="B39" s="73"/>
-      <c r="C39" s="73"/>
-      <c r="D39" s="73"/>
-      <c r="E39">
-        <v>5</v>
-      </c>
-      <c r="F39" s="64">
-        <v>3</v>
-      </c>
-      <c r="G39">
-        <v>2</v>
-      </c>
-      <c r="H39" s="62" t="s">
-        <v>24</v>
-      </c>
-      <c r="I39" s="52"/>
-      <c r="J39" s="52"/>
-      <c r="K39" s="52"/>
-    </row>
-    <row r="40" spans="1:69">
-      <c r="A40" s="73" t="s">
-        <v>64</v>
-      </c>
-      <c r="B40" s="73"/>
-      <c r="C40" s="73"/>
-      <c r="D40" s="73"/>
-      <c r="E40">
-        <v>6</v>
-      </c>
-      <c r="F40">
-        <v>4</v>
-      </c>
-      <c r="H40" s="63" t="s">
-        <v>23</v>
-      </c>
-      <c r="L40" s="57">
-        <v>5</v>
-      </c>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
-      <c r="P40" s="54"/>
-      <c r="Q40" s="54"/>
-      <c r="R40" s="54"/>
-      <c r="S40" s="54"/>
-      <c r="T40" s="54"/>
-      <c r="U40" s="54"/>
-      <c r="V40" s="54"/>
-      <c r="W40" s="54"/>
-      <c r="X40" s="54"/>
-      <c r="Y40" s="54"/>
-    </row>
-    <row r="41" spans="1:69">
-      <c r="A41" s="73" t="s">
-        <v>65</v>
-      </c>
-      <c r="B41" s="73"/>
-      <c r="C41" s="73"/>
-      <c r="D41" s="73"/>
-      <c r="E41">
-        <v>7</v>
-      </c>
-      <c r="F41">
-        <v>10</v>
-      </c>
-      <c r="H41" s="63" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z41" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA41" s="2"/>
-      <c r="AB41" s="2"/>
-      <c r="AC41" s="2"/>
-      <c r="AD41" s="2"/>
-      <c r="AE41" s="2"/>
-      <c r="AF41" s="2"/>
-      <c r="AG41" s="2"/>
-      <c r="AH41" s="2"/>
-      <c r="AI41" s="2"/>
-    </row>
-    <row r="42" spans="1:69">
-      <c r="A42" s="73" t="s">
-        <v>67</v>
-      </c>
-      <c r="B42" s="73"/>
-      <c r="C42" s="73"/>
-      <c r="D42" s="73"/>
-      <c r="E42">
-        <v>8</v>
-      </c>
-      <c r="F42">
-        <v>3</v>
-      </c>
-      <c r="H42" s="63" t="s">
-        <v>23</v>
-      </c>
-      <c r="AJ42" s="2"/>
-      <c r="AK42" s="2"/>
-      <c r="AL42" s="2"/>
-      <c r="AR42" s="59"/>
-    </row>
-    <row r="43" spans="1:69">
-      <c r="A43" s="73" t="s">
-        <v>56</v>
-      </c>
-      <c r="B43" s="73"/>
-      <c r="C43" s="73"/>
-      <c r="D43" s="73"/>
-      <c r="E43">
-        <v>9</v>
-      </c>
-      <c r="F43">
-        <v>4</v>
-      </c>
-      <c r="H43" s="63" t="s">
-        <v>23</v>
-      </c>
-      <c r="AM43" s="2"/>
-      <c r="AN43" s="2"/>
-      <c r="AO43" s="2"/>
-      <c r="AP43" s="2"/>
-      <c r="AR43" s="59"/>
-    </row>
-    <row r="44" spans="1:69">
-      <c r="A44" s="73" t="s">
-        <v>68</v>
-      </c>
-      <c r="B44" s="73"/>
-      <c r="C44" s="73"/>
-      <c r="D44" s="73"/>
-      <c r="E44">
-        <v>10</v>
-      </c>
-      <c r="F44">
-        <v>2</v>
-      </c>
-      <c r="H44" s="63" t="s">
-        <v>23</v>
-      </c>
-      <c r="AQ44" s="2"/>
-      <c r="AR44" s="57"/>
-    </row>
-    <row r="45" spans="1:69">
-      <c r="A45" s="73" t="s">
-        <v>69</v>
-      </c>
-      <c r="B45" s="73"/>
-      <c r="C45" s="73"/>
-      <c r="D45" s="73"/>
-      <c r="E45">
-        <v>11</v>
-      </c>
-      <c r="F45">
-        <v>3</v>
-      </c>
-      <c r="H45" s="63" t="s">
-        <v>23</v>
-      </c>
-      <c r="AS45" s="2"/>
-      <c r="AT45" s="2"/>
-      <c r="AU45" s="2"/>
+      <c r="AA45" s="52"/>
+      <c r="AB45" s="52"/>
+      <c r="AC45" s="52"/>
+      <c r="AD45" s="52"/>
+      <c r="AE45" s="52"/>
+      <c r="AF45" s="52"/>
+      <c r="AG45" s="52"/>
+      <c r="AH45" s="52"/>
+      <c r="AI45" s="52"/>
+      <c r="AJ45" s="52"/>
+      <c r="AK45" s="52"/>
+      <c r="AL45" s="52"/>
+      <c r="AM45" s="52"/>
+      <c r="AN45" s="52"/>
+      <c r="AO45" s="52"/>
+      <c r="AP45" s="52"/>
+      <c r="AQ45" s="52"/>
+      <c r="AR45" s="52"/>
+      <c r="AS45" s="52"/>
+      <c r="AT45" s="52"/>
     </row>
     <row r="46" spans="1:69">
       <c r="A46" s="59" t="s">
-        <v>2</v>
+        <v>52</v>
       </c>
       <c r="B46" s="59"/>
       <c r="C46" s="59"/>
       <c r="D46" s="59"/>
+      <c r="E46">
+        <v>6</v>
+      </c>
       <c r="F46">
-        <f>SUM(F35:F45)</f>
-        <v>48</v>
-      </c>
-      <c r="G46">
-        <f>SUM(G35:G45)</f>
-        <v>14</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="H46" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="AU46" s="57">
+        <v>5</v>
+      </c>
+      <c r="AV46" s="2"/>
+      <c r="AW46" s="2"/>
+      <c r="AX46" s="2"/>
+      <c r="AY46" s="2"/>
+      <c r="AZ46" s="2"/>
+      <c r="BA46" s="2"/>
     </row>
     <row r="47" spans="1:69">
-      <c r="A47" s="55" t="s">
-        <v>70</v>
-      </c>
-      <c r="B47" s="55"/>
-      <c r="C47" s="55"/>
-      <c r="D47" s="55"/>
-      <c r="E47" s="55"/>
-      <c r="F47" s="55"/>
-      <c r="G47" s="55"/>
-      <c r="H47" s="55"/>
-      <c r="I47" s="55"/>
-      <c r="J47" s="55"/>
-      <c r="K47" s="55"/>
-      <c r="L47" s="55"/>
-      <c r="M47" s="55"/>
-      <c r="N47" s="55"/>
-      <c r="O47" s="55"/>
-      <c r="P47" s="55"/>
-      <c r="Q47" s="55"/>
-      <c r="R47" s="55"/>
-      <c r="S47" s="55"/>
-      <c r="T47" s="55"/>
-      <c r="U47" s="55"/>
-      <c r="V47" s="55"/>
-      <c r="W47" s="55"/>
-      <c r="X47" s="55"/>
-      <c r="Y47" s="55"/>
-      <c r="Z47" s="55"/>
-      <c r="AA47" s="55"/>
-      <c r="AB47" s="55"/>
-      <c r="AC47" s="55"/>
-      <c r="AD47" s="55"/>
-      <c r="AE47" s="55"/>
-      <c r="AF47" s="55"/>
-      <c r="AG47" s="55"/>
-      <c r="AH47" s="55"/>
-      <c r="AI47" s="55"/>
-      <c r="AJ47" s="55"/>
-      <c r="AK47" s="55"/>
-      <c r="AL47" s="55"/>
-      <c r="AM47" s="55"/>
-      <c r="AN47" s="55"/>
-      <c r="AO47" s="55"/>
-      <c r="AP47" s="55"/>
-      <c r="AQ47" s="55"/>
-      <c r="AR47" s="55"/>
-      <c r="AS47" s="55"/>
-      <c r="AT47" s="55"/>
-      <c r="AU47" s="55"/>
-      <c r="AV47" s="55"/>
-      <c r="AW47" s="55"/>
-      <c r="AX47" s="55"/>
-      <c r="AY47" s="55"/>
-      <c r="AZ47" s="55"/>
-      <c r="BA47" s="55"/>
-      <c r="BB47" s="55"/>
-      <c r="BC47" s="55"/>
-      <c r="BD47" s="55"/>
-      <c r="BE47" s="55"/>
-      <c r="BF47" s="55"/>
-      <c r="BG47" s="55"/>
-      <c r="BH47" s="55"/>
-      <c r="BI47" s="55"/>
-      <c r="BJ47" s="55"/>
-      <c r="BK47" s="55"/>
-      <c r="BL47" s="55"/>
-      <c r="BM47" s="55"/>
+      <c r="A47" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="59"/>
+      <c r="C47" s="59"/>
+      <c r="D47" s="59"/>
+      <c r="E47">
+        <v>7</v>
+      </c>
+      <c r="F47">
+        <v>5</v>
+      </c>
+      <c r="H47" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB47" s="57">
+        <v>6</v>
+      </c>
+      <c r="BC47" s="2"/>
+      <c r="BD47" s="2"/>
+      <c r="BE47" s="2"/>
+      <c r="BF47" s="2"/>
+      <c r="BG47" s="2"/>
+      <c r="BH47" s="2"/>
       <c r="BN47" s="55"/>
       <c r="BO47" s="55"/>
       <c r="BP47" s="55"/>
@@ -2916,337 +2949,130 @@
     </row>
     <row r="48" spans="1:69">
       <c r="A48" s="59" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B48" s="59"/>
       <c r="C48" s="59"/>
       <c r="D48" s="59"/>
       <c r="E48">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="F48">
-        <v>1</v>
-      </c>
-      <c r="G48">
-        <v>1</v>
-      </c>
-      <c r="H48" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="I48" s="53"/>
+        <v>2</v>
+      </c>
+      <c r="H48" s="56" t="s">
+        <v>22</v>
+      </c>
+      <c r="BI48" s="57">
+        <v>7</v>
+      </c>
+      <c r="BJ48" s="2"/>
+      <c r="BK48" s="2"/>
+      <c r="BL48" s="2"/>
+      <c r="BM48" s="2"/>
     </row>
     <row r="49" spans="1:68">
       <c r="A49" s="59" t="s">
-        <v>72</v>
-      </c>
-      <c r="B49" s="59"/>
-      <c r="C49" s="59"/>
-      <c r="D49" s="59"/>
-      <c r="E49">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F49">
-        <v>2</v>
+        <v>66</v>
       </c>
       <c r="G49">
-        <v>2</v>
-      </c>
-      <c r="H49" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="J49" s="61">
-        <v>1</v>
-      </c>
-      <c r="K49" s="53"/>
+        <f>SUM(G41:G48)</f>
+        <v>30</v>
+      </c>
     </row>
     <row r="50" spans="1:68">
-      <c r="A50" s="59" t="s">
+      <c r="A50" s="55" t="s">
         <v>73</v>
       </c>
-      <c r="B50" s="59"/>
-      <c r="C50" s="59"/>
-      <c r="D50" s="59"/>
-      <c r="E50">
-        <v>3</v>
-      </c>
-      <c r="F50">
-        <v>14</v>
-      </c>
-      <c r="G50">
-        <v>14</v>
-      </c>
-      <c r="H50" s="53" t="s">
-        <v>25</v>
-      </c>
-      <c r="L50" s="61">
-        <v>2</v>
-      </c>
-      <c r="M50" s="53"/>
-      <c r="N50" s="53"/>
-      <c r="O50" s="53"/>
-      <c r="P50" s="53"/>
-      <c r="Q50" s="53"/>
-      <c r="R50" s="53"/>
-      <c r="S50" s="53"/>
-      <c r="T50" s="53"/>
-      <c r="U50" s="53"/>
-      <c r="V50" s="53"/>
-      <c r="W50" s="53"/>
-      <c r="X50" s="53"/>
-      <c r="Y50" s="53"/>
-    </row>
-    <row r="51" spans="1:68">
-      <c r="A51" s="59" t="s">
-        <v>74</v>
-      </c>
-      <c r="B51" s="59"/>
-      <c r="C51" s="59"/>
-      <c r="D51" s="59"/>
-      <c r="E51">
-        <v>4</v>
-      </c>
-      <c r="F51">
-        <v>12</v>
-      </c>
-      <c r="G51">
-        <v>5</v>
-      </c>
-      <c r="H51" s="52" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z51" s="58">
-        <v>3</v>
-      </c>
-      <c r="AA51" s="52"/>
-      <c r="AB51" s="52"/>
-      <c r="AC51" s="52"/>
-      <c r="AD51" s="52"/>
-      <c r="AE51" s="52"/>
-      <c r="AF51" s="52"/>
-      <c r="AG51" s="52"/>
-      <c r="AH51" s="52"/>
-      <c r="AI51" s="52"/>
-      <c r="AJ51" s="52"/>
-      <c r="AK51" s="52"/>
-    </row>
-    <row r="52" spans="1:68">
-      <c r="A52" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="B52" s="59"/>
-      <c r="C52" s="59"/>
-      <c r="D52" s="59"/>
-      <c r="E52">
-        <v>5</v>
-      </c>
-      <c r="F52">
-        <v>23</v>
-      </c>
-      <c r="G52">
-        <v>8</v>
-      </c>
-      <c r="H52" s="52" t="s">
-        <v>24</v>
-      </c>
-      <c r="Z52" s="58">
-        <v>3</v>
-      </c>
-      <c r="AA52" s="52"/>
-      <c r="AB52" s="52"/>
-      <c r="AC52" s="52"/>
-      <c r="AD52" s="52"/>
-      <c r="AE52" s="52"/>
-      <c r="AF52" s="52"/>
-      <c r="AG52" s="52"/>
-      <c r="AH52" s="52"/>
-      <c r="AI52" s="52"/>
-      <c r="AJ52" s="52"/>
-      <c r="AK52" s="52"/>
-      <c r="AL52" s="52"/>
-      <c r="AM52" s="52"/>
-      <c r="AN52" s="52"/>
-      <c r="AO52" s="52"/>
-      <c r="AP52" s="52"/>
-      <c r="AQ52" s="52"/>
-      <c r="AR52" s="52"/>
-      <c r="AS52" s="52"/>
-      <c r="AT52" s="52"/>
-    </row>
-    <row r="53" spans="1:68">
-      <c r="A53" s="59" t="s">
-        <v>56</v>
-      </c>
-      <c r="B53" s="59"/>
-      <c r="C53" s="59"/>
-      <c r="D53" s="59"/>
-      <c r="E53">
-        <v>6</v>
-      </c>
-      <c r="F53">
-        <v>7</v>
-      </c>
-      <c r="H53" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="AU53" s="57">
-        <v>5</v>
-      </c>
-      <c r="AV53" s="2"/>
-      <c r="AW53" s="2"/>
-      <c r="AX53" s="2"/>
-      <c r="AY53" s="2"/>
-      <c r="AZ53" s="2"/>
-      <c r="BA53" s="2"/>
-    </row>
-    <row r="54" spans="1:68">
-      <c r="A54" s="59" t="s">
-        <v>76</v>
-      </c>
-      <c r="B54" s="59"/>
-      <c r="C54" s="59"/>
-      <c r="D54" s="59"/>
-      <c r="E54">
-        <v>7</v>
-      </c>
-      <c r="F54">
-        <v>5</v>
-      </c>
-      <c r="H54" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="BB54" s="57">
-        <v>6</v>
-      </c>
-      <c r="BC54" s="2"/>
-      <c r="BD54" s="2"/>
-      <c r="BE54" s="2"/>
-      <c r="BF54" s="2"/>
-      <c r="BG54" s="2"/>
-      <c r="BH54" s="2"/>
-    </row>
-    <row r="55" spans="1:68">
-      <c r="A55" s="59" t="s">
-        <v>77</v>
-      </c>
-      <c r="B55" s="59"/>
-      <c r="C55" s="59"/>
-      <c r="D55" s="59"/>
-      <c r="E55">
-        <v>8</v>
-      </c>
-      <c r="F55">
-        <v>2</v>
-      </c>
-      <c r="H55" s="56" t="s">
-        <v>23</v>
-      </c>
-      <c r="BI55" s="57">
-        <v>7</v>
-      </c>
-      <c r="BJ55" s="2"/>
-      <c r="BK55" s="2"/>
-      <c r="BL55" s="2"/>
-      <c r="BM55" s="2"/>
-    </row>
-    <row r="56" spans="1:68">
-      <c r="A56" s="59" t="s">
-        <v>2</v>
-      </c>
-      <c r="F56">
-        <v>66</v>
-      </c>
-      <c r="G56">
-        <f>SUM(G48:G55)</f>
-        <v>30</v>
-      </c>
+      <c r="B50" s="55"/>
+      <c r="C50" s="55"/>
+      <c r="D50" s="55"/>
+      <c r="E50" s="55"/>
+      <c r="F50" s="55"/>
+      <c r="G50" s="55"/>
+      <c r="H50" s="55"/>
+      <c r="I50" s="55"/>
+      <c r="J50" s="55"/>
+      <c r="K50" s="55"/>
+      <c r="L50" s="55"/>
+      <c r="M50" s="55"/>
+      <c r="N50" s="55"/>
+      <c r="O50" s="55"/>
+      <c r="P50" s="55"/>
+      <c r="Q50" s="55"/>
+      <c r="R50" s="55"/>
+      <c r="S50" s="55"/>
+      <c r="T50" s="55"/>
+      <c r="U50" s="55"/>
+      <c r="V50" s="55"/>
+      <c r="W50" s="55"/>
+      <c r="X50" s="55"/>
+      <c r="Y50" s="55"/>
+      <c r="Z50" s="55"/>
+      <c r="AA50" s="55"/>
+      <c r="AB50" s="55"/>
+      <c r="AC50" s="55"/>
+      <c r="AD50" s="55"/>
+      <c r="AE50" s="55"/>
+      <c r="AF50" s="55"/>
+      <c r="AG50" s="55"/>
+      <c r="AH50" s="55"/>
+      <c r="AI50" s="55"/>
+      <c r="AJ50" s="55"/>
+      <c r="AK50" s="55"/>
+      <c r="AL50" s="55"/>
+      <c r="AM50" s="55"/>
+      <c r="AN50" s="55"/>
+      <c r="AO50" s="55"/>
+      <c r="AP50" s="55"/>
+      <c r="AQ50" s="55"/>
+      <c r="AR50" s="55"/>
+      <c r="AS50" s="55"/>
+      <c r="AT50" s="55"/>
+      <c r="AU50" s="55"/>
+      <c r="AV50" s="55"/>
+      <c r="AW50" s="55"/>
+      <c r="AX50" s="55"/>
+      <c r="AY50" s="55"/>
+      <c r="AZ50" s="55"/>
+      <c r="BA50" s="55"/>
+      <c r="BB50" s="55"/>
+      <c r="BC50" s="55"/>
+      <c r="BD50" s="55"/>
+      <c r="BE50" s="55"/>
+      <c r="BF50" s="55"/>
+      <c r="BG50" s="55"/>
+      <c r="BH50" s="55"/>
+      <c r="BI50" s="55"/>
+      <c r="BJ50" s="55"/>
+      <c r="BK50" s="55"/>
+      <c r="BL50" s="55"/>
+      <c r="BM50" s="55"/>
     </row>
     <row r="57" spans="1:68">
-      <c r="A57" s="55" t="s">
-        <v>78</v>
-      </c>
-      <c r="B57" s="55"/>
-      <c r="C57" s="55"/>
-      <c r="D57" s="55"/>
-      <c r="E57" s="55"/>
-      <c r="F57" s="55"/>
-      <c r="G57" s="55"/>
-      <c r="H57" s="55"/>
-      <c r="I57" s="55"/>
-      <c r="J57" s="55"/>
-      <c r="K57" s="55"/>
-      <c r="L57" s="55"/>
-      <c r="M57" s="55"/>
-      <c r="N57" s="55"/>
-      <c r="O57" s="55"/>
-      <c r="P57" s="55"/>
-      <c r="Q57" s="55"/>
-      <c r="R57" s="55"/>
-      <c r="S57" s="55"/>
-      <c r="T57" s="55"/>
-      <c r="U57" s="55"/>
-      <c r="V57" s="55"/>
-      <c r="W57" s="55"/>
-      <c r="X57" s="55"/>
-      <c r="Y57" s="55"/>
-      <c r="Z57" s="55"/>
-      <c r="AA57" s="55"/>
-      <c r="AB57" s="55"/>
-      <c r="AC57" s="55"/>
-      <c r="AD57" s="55"/>
-      <c r="AE57" s="55"/>
-      <c r="AF57" s="55"/>
-      <c r="AG57" s="55"/>
-      <c r="AH57" s="55"/>
-      <c r="AI57" s="55"/>
-      <c r="AJ57" s="55"/>
-      <c r="AK57" s="55"/>
-      <c r="AL57" s="55"/>
-      <c r="AM57" s="55"/>
-      <c r="AN57" s="55"/>
-      <c r="AO57" s="55"/>
-      <c r="AP57" s="55"/>
-      <c r="AQ57" s="55"/>
-      <c r="AR57" s="55"/>
-      <c r="AS57" s="55"/>
-      <c r="AT57" s="55"/>
-      <c r="AU57" s="55"/>
-      <c r="AV57" s="55"/>
-      <c r="AW57" s="55"/>
-      <c r="AX57" s="55"/>
-      <c r="AY57" s="55"/>
-      <c r="AZ57" s="55"/>
-      <c r="BA57" s="55"/>
-      <c r="BB57" s="55"/>
-      <c r="BC57" s="55"/>
-      <c r="BD57" s="55"/>
-      <c r="BE57" s="55"/>
-      <c r="BF57" s="55"/>
-      <c r="BG57" s="55"/>
-      <c r="BH57" s="55"/>
-      <c r="BI57" s="55"/>
-      <c r="BJ57" s="55"/>
-      <c r="BK57" s="55"/>
-      <c r="BL57" s="55"/>
-      <c r="BM57" s="55"/>
       <c r="BN57" s="55"/>
       <c r="BO57" s="55"/>
       <c r="BP57" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="A33:D33"/>
+    <mergeCell ref="A34:D34"/>
     <mergeCell ref="A35:D35"/>
     <mergeCell ref="A36:D36"/>
     <mergeCell ref="A37:D37"/>
-    <mergeCell ref="A38:D38"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A39:D39"/>
-    <mergeCell ref="A40:D40"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A43:D43"/>
-    <mergeCell ref="A44:D44"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3258,26 +3084,26 @@
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="B1" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>84</v>
-      </c>
       <c r="G1" s="5" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
@@ -3287,22 +3113,22 @@
     </row>
     <row r="2" spans="1:12" ht="62.25" customHeight="1">
       <c r="B2" s="5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
@@ -3312,7 +3138,7 @@
     </row>
     <row r="3" spans="1:12">
       <c r="B3" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C3" s="5">
         <v>1</v>
@@ -3347,21 +3173,21 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" s="5" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B4" s="5">
         <f>SUMIF(C4:L4,A$10,C$3:Z$3)</f>
         <v>6</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
@@ -3372,23 +3198,23 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" s="5" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B5" s="5">
         <f>SUMIF(C5:L5,A$10,C$3:Z$3)</f>
         <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G5" s="4"/>
       <c r="J5" s="4"/>
@@ -3397,23 +3223,23 @@
     </row>
     <row r="6" spans="1:12">
       <c r="A6" s="5" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B6" s="5">
         <f>SUMIF(C6:L6,A$10,C$3:Z$3)</f>
         <v>9</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
@@ -3424,23 +3250,23 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="5" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B7" s="5">
         <f>SUMIF(C7:L7,A$10,C$3:Z$3)</f>
         <v>9</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="4"/>
@@ -3451,7 +3277,7 @@
     </row>
     <row r="8" spans="1:12">
       <c r="A8" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B8" s="7">
         <f>SUM(B4:B7)</f>
@@ -3503,7 +3329,7 @@
     </row>
     <row r="10" spans="1:12">
       <c r="A10" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:12">
@@ -3523,25 +3349,25 @@
       <selection activeCell="G29" activeCellId="1" sqref="G28 G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
     <col min="2" max="2" width="29.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.5" customWidth="1"/>
-    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="14.44140625" customWidth="1"/>
+    <col min="4" max="4" width="10.44140625" customWidth="1"/>
     <col min="5" max="19" width="3.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="32"/>
       <c r="B1" s="33" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="34" t="s">
         <v>12</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="34" t="s">
-        <v>13</v>
       </c>
       <c r="E1">
         <v>1</v>
@@ -3591,10 +3417,10 @@
     </row>
     <row r="2" spans="1:19">
       <c r="A2" s="35" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B2" s="36" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C2" s="37">
         <v>2</v>
@@ -3608,7 +3434,7 @@
     <row r="3" spans="1:19">
       <c r="A3" s="46"/>
       <c r="B3" s="36" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C3" s="37">
         <v>2</v>
@@ -3627,7 +3453,7 @@
     <row r="4" spans="1:19">
       <c r="A4" s="39"/>
       <c r="B4" s="36" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C4" s="37">
         <v>10</v>
@@ -3636,7 +3462,7 @@
         <v>3</v>
       </c>
       <c r="G4" s="69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
@@ -3651,7 +3477,7 @@
     </row>
     <row r="5" spans="1:19">
       <c r="B5" s="36" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C5" s="66">
         <v>6</v>
@@ -3660,7 +3486,7 @@
         <v>2</v>
       </c>
       <c r="G5" s="69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3"/>
@@ -3671,7 +3497,7 @@
     </row>
     <row r="6" spans="1:19">
       <c r="B6" s="36" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C6" s="66">
         <v>5</v>
@@ -3680,7 +3506,7 @@
         <v>2</v>
       </c>
       <c r="G6" s="69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3"/>
@@ -3690,7 +3516,7 @@
     </row>
     <row r="7" spans="1:19">
       <c r="B7" s="36" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C7" s="66">
         <v>5</v>
@@ -3699,7 +3525,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
@@ -3709,7 +3535,7 @@
     <row r="8" spans="1:19">
       <c r="A8" s="39"/>
       <c r="B8" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8" s="36">
         <f>SUM(C2:C7)</f>
@@ -3722,10 +3548,10 @@
     </row>
     <row r="9" spans="1:19">
       <c r="A9" s="35" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C9" s="37">
         <v>2</v>
@@ -3739,7 +3565,7 @@
     <row r="10" spans="1:19">
       <c r="A10" s="46"/>
       <c r="B10" s="36" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C10" s="66">
         <v>2</v>
@@ -3758,7 +3584,7 @@
     <row r="11" spans="1:19">
       <c r="A11" s="39"/>
       <c r="B11" s="36" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C11" s="66">
         <v>10</v>
@@ -3769,7 +3595,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -3786,7 +3612,7 @@
     </row>
     <row r="12" spans="1:19">
       <c r="B12" s="36" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C12" s="66">
         <v>6</v>
@@ -3797,7 +3623,7 @@
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H12" s="30"/>
       <c r="I12" s="30"/>
@@ -3814,7 +3640,7 @@
     </row>
     <row r="13" spans="1:19">
       <c r="B13" s="36" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C13" s="66">
         <v>5</v>
@@ -3825,7 +3651,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -3842,7 +3668,7 @@
     </row>
     <row r="14" spans="1:19">
       <c r="B14" s="36" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C14" s="66">
         <v>10</v>
@@ -3853,7 +3679,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -3871,7 +3697,7 @@
     <row r="15" spans="1:19">
       <c r="A15" s="39"/>
       <c r="B15" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="36">
         <f>SUM(C9:C14)</f>
@@ -3899,7 +3725,7 @@
     </row>
     <row r="16" spans="1:19">
       <c r="A16" s="35" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="B16" s="36"/>
       <c r="C16" s="37"/>
@@ -3923,7 +3749,7 @@
     <row r="17" spans="1:19">
       <c r="A17" s="46"/>
       <c r="B17" s="36" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C17" s="66">
         <v>2</v>
@@ -3950,7 +3776,7 @@
     <row r="18" spans="1:19">
       <c r="A18" s="39"/>
       <c r="B18" s="67" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C18" s="66">
         <v>2</v>
@@ -3965,7 +3791,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
       <c r="K18" s="65" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
@@ -3979,7 +3805,7 @@
     <row r="19" spans="1:19">
       <c r="A19" s="39"/>
       <c r="B19" s="68" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C19" s="37">
         <v>10</v>
@@ -3990,7 +3816,7 @@
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3"/>
@@ -4008,7 +3834,7 @@
     <row r="20" spans="1:19">
       <c r="A20" s="39"/>
       <c r="B20" s="67" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C20" s="66">
         <v>6</v>
@@ -4019,7 +3845,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -4036,7 +3862,7 @@
     </row>
     <row r="21" spans="1:19">
       <c r="B21" s="68" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C21" s="66">
         <v>5</v>
@@ -4047,7 +3873,7 @@
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
@@ -4064,7 +3890,7 @@
     </row>
     <row r="22" spans="1:19">
       <c r="B22" s="67" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C22">
         <v>8</v>
@@ -4075,7 +3901,7 @@
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
       <c r="G22" s="69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
@@ -4093,7 +3919,7 @@
     <row r="23" spans="1:19">
       <c r="A23" s="39"/>
       <c r="B23" s="41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C23" s="36">
         <f>SUM(C17:C22)</f>
@@ -4121,10 +3947,10 @@
     </row>
     <row r="24" spans="1:19">
       <c r="A24" s="35" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C24" s="37">
         <v>2</v>
@@ -4151,7 +3977,7 @@
     <row r="25" spans="1:19">
       <c r="A25" s="46"/>
       <c r="B25" s="36" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C25" s="66">
         <v>2</v>
@@ -4178,7 +4004,7 @@
     <row r="26" spans="1:19">
       <c r="A26" s="39"/>
       <c r="B26" s="36" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C26" s="66">
         <v>10</v>
@@ -4189,7 +4015,7 @@
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
       <c r="G26" s="69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -4206,7 +4032,7 @@
     </row>
     <row r="27" spans="1:19">
       <c r="B27" s="36" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C27" s="66">
         <v>6</v>
@@ -4217,7 +4043,7 @@
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
@@ -4234,7 +4060,7 @@
     </row>
     <row r="28" spans="1:19">
       <c r="B28" s="36" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C28" s="66">
         <v>5</v>
@@ -4245,7 +4071,7 @@
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H28" s="3"/>
       <c r="I28" s="3"/>
@@ -4262,7 +4088,7 @@
     </row>
     <row r="29" spans="1:19">
       <c r="B29" s="36" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C29">
         <v>10</v>
@@ -4271,7 +4097,7 @@
         <v>5</v>
       </c>
       <c r="G29" s="69" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3"/>
@@ -4287,7 +4113,7 @@
     <row r="30" spans="1:19">
       <c r="A30" s="39"/>
       <c r="B30" s="41" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30" s="36">
         <f>SUM(C24:C29)</f>
@@ -4298,10 +4124,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:19" ht="16" thickBot="1">
+    <row r="31" spans="1:19" ht="15" thickBot="1">
       <c r="A31" s="42"/>
       <c r="B31" s="43" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C31" s="44">
         <f>SUM(C8,C15,C23,C30)</f>
@@ -4314,7 +4140,7 @@
     </row>
     <row r="32" spans="1:19">
       <c r="B32" s="31" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -4331,28 +4157,28 @@
       <selection activeCell="G14" sqref="G14:G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D1" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E1" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F1" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G1" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:9">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D2">
         <v>5</v>
@@ -4369,7 +4195,7 @@
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D3">
         <v>3</v>
@@ -4386,7 +4212,7 @@
     </row>
     <row r="4" spans="1:9">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D4">
         <v>5</v>
@@ -4403,7 +4229,7 @@
     </row>
     <row r="5" spans="1:9">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D5">
         <v>5</v>
@@ -4418,12 +4244,12 @@
         <v>3</v>
       </c>
       <c r="I5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D6">
         <v>3</v>
@@ -4440,7 +4266,7 @@
     </row>
     <row r="7" spans="1:9">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D7">
         <v>3</v>
@@ -4457,7 +4283,7 @@
     </row>
     <row r="8" spans="1:9">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D8">
         <f>SUM(D2:D7)</f>
@@ -4478,24 +4304,24 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D13" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="E13" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="F13" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G13" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D14">
         <v>3</v>
@@ -4512,7 +4338,7 @@
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="D15">
         <v>2</v>
@@ -4529,7 +4355,7 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D16">
         <v>3</v>
@@ -4544,12 +4370,12 @@
         <v>0</v>
       </c>
       <c r="I16" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D17">
         <v>3</v>
@@ -4566,7 +4392,7 @@
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -4583,7 +4409,7 @@
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -4600,7 +4426,7 @@
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D20">
         <f>SUM(D14:D19)</f>

</xml_diff>